<commit_message>
See var distribution across groups
</commit_message>
<xml_diff>
--- a/00_Data/DF EOF Projects Overview (2004-2023).xlsx
+++ b/00_Data/DF EOF Projects Overview (2004-2023).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/zchen2545_wisc_edu/Documents/Research/Discovery Farms/DF Runoff Generation/Github repo/DF_runoff/00_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_19408F433B3B1D7D2F1C74842EF54AAEDA41FF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_19408F433B3B1D7D2F1C74842EF54AAEDA41FF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9385DEF6-39F5-4862-A7AF-F22AA82A8DAF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WI" sheetId="1" r:id="rId1"/>
@@ -2690,25 +2690,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2722,14 +2712,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2956,8 +2956,8 @@
   </sheetPr>
   <dimension ref="A1:AD1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3032,19 +3032,19 @@
       <c r="AD1" s="6"/>
     </row>
     <row r="2" spans="1:30" ht="13.2">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="98" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -3086,11 +3086,11 @@
       <c r="AD2" s="12"/>
     </row>
     <row r="3" spans="1:30" ht="13.2">
-      <c r="A3" s="88"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
+      <c r="A3" s="89"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
       <c r="F3" s="13" t="s">
         <v>23</v>
       </c>
@@ -3240,19 +3240,19 @@
       <c r="AD5" s="12"/>
     </row>
     <row r="6" spans="1:30" ht="13.2">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="87" t="s">
+      <c r="C6" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="93" t="s">
+      <c r="E6" s="101" t="s">
         <v>43</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -3296,11 +3296,11 @@
       <c r="AD6" s="12"/>
     </row>
     <row r="7" spans="1:30" ht="13.2">
-      <c r="A7" s="92"/>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
       <c r="F7" s="21" t="s">
         <v>49</v>
       </c>
@@ -3340,11 +3340,11 @@
       <c r="AD7" s="12"/>
     </row>
     <row r="8" spans="1:30" ht="13.2">
-      <c r="A8" s="92"/>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="21" t="s">
         <v>51</v>
       </c>
@@ -3386,11 +3386,11 @@
       <c r="AD8" s="12"/>
     </row>
     <row r="9" spans="1:30" ht="13.2">
-      <c r="A9" s="92"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
       <c r="F9" s="21" t="s">
         <v>53</v>
       </c>
@@ -3432,11 +3432,11 @@
       <c r="AD9" s="12"/>
     </row>
     <row r="10" spans="1:30" ht="13.2">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="23" t="s">
         <v>57</v>
       </c>
@@ -3478,19 +3478,19 @@
       <c r="AD10" s="12"/>
     </row>
     <row r="11" spans="1:30" ht="13.2">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="90" t="s">
+      <c r="D11" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="93" t="s">
+      <c r="E11" s="101" t="s">
         <v>62</v>
       </c>
       <c r="F11" s="10" t="s">
@@ -3532,11 +3532,11 @@
       <c r="AD11" s="12"/>
     </row>
     <row r="12" spans="1:30" ht="13.2">
-      <c r="A12" s="92"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
       <c r="F12" s="21" t="s">
         <v>65</v>
       </c>
@@ -3576,11 +3576,11 @@
       <c r="AD12" s="12"/>
     </row>
     <row r="13" spans="1:30" ht="13.2">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
       <c r="F13" s="23" t="s">
         <v>66</v>
       </c>
@@ -3620,19 +3620,19 @@
       <c r="AD13" s="12"/>
     </row>
     <row r="14" spans="1:30" ht="52.8">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="90" t="s">
+      <c r="D14" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="91" t="s">
+      <c r="E14" s="98" t="s">
         <v>70</v>
       </c>
       <c r="F14" s="10" t="s">
@@ -3676,11 +3676,11 @@
       <c r="AD14" s="12"/>
     </row>
     <row r="15" spans="1:30" ht="13.2">
-      <c r="A15" s="92"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
       <c r="F15" s="21" t="s">
         <v>75</v>
       </c>
@@ -3720,11 +3720,11 @@
       <c r="AD15" s="12"/>
     </row>
     <row r="16" spans="1:30" ht="13.2">
-      <c r="A16" s="88"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
       <c r="F16" s="23" t="s">
         <v>77</v>
       </c>
@@ -3764,19 +3764,19 @@
       <c r="AD16" s="12"/>
     </row>
     <row r="17" spans="1:30" ht="13.2">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="90" t="s">
+      <c r="D17" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="93" t="s">
+      <c r="E17" s="101" t="s">
         <v>81</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -3820,11 +3820,11 @@
       <c r="AD17" s="12"/>
     </row>
     <row r="18" spans="1:30" ht="13.2">
-      <c r="A18" s="92"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
       <c r="F18" s="21" t="s">
         <v>86</v>
       </c>
@@ -3866,11 +3866,11 @@
       <c r="AD18" s="12"/>
     </row>
     <row r="19" spans="1:30" ht="13.2">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
       <c r="F19" s="14" t="s">
         <v>87</v>
       </c>
@@ -3910,16 +3910,16 @@
       <c r="AD19" s="12"/>
     </row>
     <row r="20" spans="1:30" ht="13.2">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="95" t="s">
+      <c r="D20" s="97" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -3966,10 +3966,10 @@
       <c r="AD20" s="12"/>
     </row>
     <row r="21" spans="1:30" ht="13.2">
-      <c r="A21" s="92"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
       <c r="E21" s="8" t="s">
         <v>96</v>
       </c>
@@ -4014,10 +4014,10 @@
       <c r="AD21" s="12"/>
     </row>
     <row r="22" spans="1:30" ht="13.2">
-      <c r="A22" s="92"/>
-      <c r="B22" s="92"/>
-      <c r="C22" s="92"/>
-      <c r="D22" s="92"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
       <c r="E22" s="8" t="s">
         <v>99</v>
       </c>
@@ -4060,10 +4060,10 @@
       <c r="AD22" s="12"/>
     </row>
     <row r="23" spans="1:30" ht="13.2">
-      <c r="A23" s="92"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
+      <c r="A23" s="88"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
       <c r="E23" s="7"/>
       <c r="F23" s="21" t="s">
         <v>101</v>
@@ -4104,10 +4104,10 @@
       <c r="AD23" s="12"/>
     </row>
     <row r="24" spans="1:30" ht="13.2">
-      <c r="A24" s="92"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
       <c r="E24" s="7"/>
       <c r="F24" s="21" t="s">
         <v>103</v>
@@ -4150,10 +4150,10 @@
       <c r="AD24" s="12"/>
     </row>
     <row r="25" spans="1:30" ht="24" customHeight="1">
-      <c r="A25" s="88"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
       <c r="E25" s="14"/>
       <c r="F25" s="23" t="s">
         <v>105</v>
@@ -4205,10 +4205,10 @@
       <c r="C26" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="90" t="s">
+      <c r="D26" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="91" t="s">
+      <c r="E26" s="98" t="s">
         <v>109</v>
       </c>
       <c r="F26" s="10" t="s">
@@ -4261,8 +4261,8 @@
       <c r="C27" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
       <c r="F27" s="21" t="s">
         <v>117</v>
       </c>
@@ -4311,8 +4311,8 @@
       <c r="C28" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
       <c r="F28" s="21" t="s">
         <v>120</v>
       </c>
@@ -4361,8 +4361,8 @@
       <c r="C29" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D29" s="92"/>
-      <c r="E29" s="92"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
       <c r="F29" s="21" t="s">
         <v>125</v>
       </c>
@@ -4411,8 +4411,8 @@
       <c r="C30" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
       <c r="F30" s="21" t="s">
         <v>128</v>
       </c>
@@ -4461,8 +4461,8 @@
       <c r="C31" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
       <c r="F31" s="23" t="s">
         <v>131</v>
       </c>
@@ -4511,10 +4511,10 @@
       <c r="C32" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D32" s="90" t="s">
+      <c r="D32" s="91" t="s">
         <v>137</v>
       </c>
-      <c r="E32" s="91" t="s">
+      <c r="E32" s="98" t="s">
         <v>109</v>
       </c>
       <c r="F32" s="10" t="s">
@@ -4565,8 +4565,8 @@
       <c r="C33" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="92"/>
-      <c r="E33" s="92"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
       <c r="F33" s="21" t="s">
         <v>141</v>
       </c>
@@ -4617,8 +4617,8 @@
       <c r="C34" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
       <c r="F34" s="23" t="s">
         <v>146</v>
       </c>
@@ -4658,16 +4658,16 @@
       <c r="AD34" s="12"/>
     </row>
     <row r="35" spans="1:30" ht="13.2">
-      <c r="A35" s="87" t="s">
+      <c r="A35" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="87" t="s">
+      <c r="B35" s="90" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="87" t="s">
+      <c r="C35" s="90" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="90" t="s">
+      <c r="D35" s="91" t="s">
         <v>150</v>
       </c>
       <c r="E35" s="8" t="s">
@@ -4712,10 +4712,10 @@
       <c r="AD35" s="12"/>
     </row>
     <row r="36" spans="1:30" ht="13.2">
-      <c r="A36" s="88"/>
-      <c r="B36" s="88"/>
-      <c r="C36" s="88"/>
-      <c r="D36" s="88"/>
+      <c r="A36" s="89"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
       <c r="E36" s="18" t="s">
         <v>154</v>
       </c>
@@ -4758,16 +4758,16 @@
       <c r="AD36" s="12"/>
     </row>
     <row r="37" spans="1:30" ht="13.2">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="87" t="s">
+      <c r="B37" s="90" t="s">
         <v>156</v>
       </c>
-      <c r="C37" s="87" t="s">
+      <c r="C37" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="D37" s="97" t="s">
+      <c r="D37" s="93" t="s">
         <v>158</v>
       </c>
       <c r="E37" s="8" t="s">
@@ -4812,10 +4812,10 @@
       <c r="AD37" s="12"/>
     </row>
     <row r="38" spans="1:30" ht="13.2">
-      <c r="A38" s="88"/>
-      <c r="B38" s="88"/>
-      <c r="C38" s="88"/>
-      <c r="D38" s="98"/>
+      <c r="A38" s="89"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="94"/>
       <c r="E38" s="8" t="s">
         <v>161</v>
       </c>
@@ -4867,7 +4867,7 @@
       <c r="C39" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D39" s="99" t="s">
+      <c r="D39" s="95" t="s">
         <v>165</v>
       </c>
       <c r="E39" s="36" t="s">
@@ -4891,7 +4891,7 @@
       <c r="K39" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="L39" s="101"/>
+      <c r="L39" s="87"/>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
@@ -4921,7 +4921,7 @@
       <c r="C40" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="D40" s="100"/>
+      <c r="D40" s="96"/>
       <c r="E40" s="8" t="s">
         <v>171</v>
       </c>
@@ -4943,7 +4943,7 @@
       <c r="K40" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L40" s="92"/>
+      <c r="L40" s="88"/>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
       <c r="O40" s="12"/>
@@ -4973,7 +4973,7 @@
       <c r="C41" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D41" s="98"/>
+      <c r="D41" s="94"/>
       <c r="E41" s="14"/>
       <c r="F41" s="35" t="s">
         <v>175</v>
@@ -4993,7 +4993,7 @@
       <c r="K41" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L41" s="88"/>
+      <c r="L41" s="89"/>
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
       <c r="O41" s="12"/>
@@ -5014,16 +5014,16 @@
       <c r="AD41" s="12"/>
     </row>
     <row r="42" spans="1:30" ht="13.2">
-      <c r="A42" s="87" t="s">
+      <c r="A42" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C42" s="90" t="s">
+      <c r="C42" s="91" t="s">
         <v>177</v>
       </c>
-      <c r="D42" s="96" t="s">
+      <c r="D42" s="92" t="s">
         <v>178</v>
       </c>
       <c r="E42" s="8" t="s">
@@ -5068,12 +5068,12 @@
       <c r="AD42" s="12"/>
     </row>
     <row r="43" spans="1:30" ht="13.2">
-      <c r="A43" s="88"/>
+      <c r="A43" s="89"/>
       <c r="B43" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="C43" s="88"/>
-      <c r="D43" s="88"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
       <c r="E43" s="18" t="s">
         <v>183</v>
       </c>
@@ -5116,7 +5116,7 @@
       <c r="AD43" s="12"/>
     </row>
     <row r="44" spans="1:30" ht="52.8">
-      <c r="A44" s="87" t="s">
+      <c r="A44" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="10" t="s">
@@ -5170,7 +5170,7 @@
       <c r="AD44" s="12"/>
     </row>
     <row r="45" spans="1:30" ht="52.8">
-      <c r="A45" s="88"/>
+      <c r="A45" s="89"/>
       <c r="B45" s="23" t="s">
         <v>191</v>
       </c>
@@ -5224,7 +5224,7 @@
       <c r="AD45" s="12"/>
     </row>
     <row r="46" spans="1:30" ht="26.4">
-      <c r="A46" s="87" t="s">
+      <c r="A46" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="10" t="s">
@@ -5278,7 +5278,7 @@
       <c r="AD46" s="12"/>
     </row>
     <row r="47" spans="1:30" ht="26.4">
-      <c r="A47" s="92"/>
+      <c r="A47" s="88"/>
       <c r="B47" s="21" t="s">
         <v>202</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="AD47" s="12"/>
     </row>
     <row r="48" spans="1:30" ht="39.6">
-      <c r="A48" s="88"/>
+      <c r="A48" s="89"/>
       <c r="B48" s="23" t="s">
         <v>206</v>
       </c>
@@ -5380,7 +5380,7 @@
       <c r="AD48" s="12"/>
     </row>
     <row r="49" spans="1:30" ht="39.6">
-      <c r="A49" s="87" t="s">
+      <c r="A49" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B49" s="10" t="s">
@@ -5434,7 +5434,7 @@
       <c r="AD49" s="12"/>
     </row>
     <row r="50" spans="1:30" ht="39.6">
-      <c r="A50" s="92"/>
+      <c r="A50" s="88"/>
       <c r="B50" s="21" t="s">
         <v>216</v>
       </c>
@@ -5484,7 +5484,7 @@
       <c r="AD50" s="12"/>
     </row>
     <row r="51" spans="1:30" ht="26.4">
-      <c r="A51" s="94"/>
+      <c r="A51" s="99"/>
       <c r="B51" s="21" t="s">
         <v>221</v>
       </c>
@@ -36381,38 +36381,11 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="L39:L41"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="C17:C19"/>
@@ -36425,11 +36398,38 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="E14:E16"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="L39:L41"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -36522,16 +36522,16 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="90" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="90" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="91" t="s">
         <v>229</v>
       </c>
       <c r="E2" s="46" t="s">
@@ -36558,10 +36558,10 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="92"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
       <c r="E3" s="46" t="s">
         <v>235</v>
       </c>
@@ -36586,10 +36586,10 @@
       <c r="L3" s="49"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
+      <c r="A4" s="89"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="50"/>
       <c r="F4" s="23" t="s">
         <v>237</v>
@@ -36612,16 +36612,16 @@
       <c r="L4" s="51"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="90" t="s">
         <v>238</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="90" t="s">
         <v>239</v>
       </c>
-      <c r="D5" s="90" t="s">
+      <c r="D5" s="91" t="s">
         <v>240</v>
       </c>
       <c r="E5" s="52" t="s">
@@ -36650,10 +36650,10 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="46" t="s">
         <v>244</v>
       </c>
@@ -36752,16 +36752,16 @@
       <c r="L8" s="50"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="90" t="s">
         <v>258</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="90" t="s">
         <v>259</v>
       </c>
-      <c r="D9" s="90" t="s">
+      <c r="D9" s="91" t="s">
         <v>260</v>
       </c>
       <c r="E9" s="52" t="s">
@@ -36790,10 +36790,10 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="55" t="s">
         <v>264</v>
       </c>
@@ -36858,16 +36858,16 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="90" t="s">
         <v>275</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="C12" s="103" t="s">
         <v>276</v>
       </c>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="104" t="s">
         <v>277</v>
       </c>
       <c r="E12" s="46" t="s">
@@ -36896,10 +36896,10 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
       <c r="E13" s="58" t="s">
         <v>281</v>
       </c>
@@ -36962,16 +36962,16 @@
       <c r="L14" s="50"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="90" t="s">
         <v>290</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="90" t="s">
         <v>291</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="91" t="s">
         <v>292</v>
       </c>
       <c r="E15" s="46" t="s">
@@ -37000,10 +37000,10 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="88"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
       <c r="E16" s="61" t="s">
         <v>296</v>
       </c>
@@ -37064,16 +37064,16 @@
       <c r="L17" s="50"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="90" t="s">
         <v>305</v>
       </c>
-      <c r="C18" s="87" t="s">
+      <c r="C18" s="90" t="s">
         <v>306</v>
       </c>
-      <c r="D18" s="90" t="s">
+      <c r="D18" s="91" t="s">
         <v>307</v>
       </c>
       <c r="E18" s="52" t="s">
@@ -37102,10 +37102,10 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
       <c r="E19" s="55" t="s">
         <v>311</v>
       </c>
@@ -37132,16 +37132,16 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="90" t="s">
         <v>314</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="90" t="s">
         <v>315</v>
       </c>
-      <c r="D20" s="97" t="s">
+      <c r="D20" s="93" t="s">
         <v>316</v>
       </c>
       <c r="E20" s="46" t="s">
@@ -37170,10 +37170,10 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="88"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="98"/>
+      <c r="A21" s="89"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="94"/>
       <c r="E21" s="50"/>
       <c r="F21" s="59" t="s">
         <v>321</v>
@@ -37198,16 +37198,16 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="90" t="s">
         <v>323</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="90" t="s">
         <v>324</v>
       </c>
-      <c r="D22" s="97" t="s">
+      <c r="D22" s="93" t="s">
         <v>325</v>
       </c>
       <c r="E22" s="52" t="s">
@@ -37236,10 +37236,10 @@
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="92"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="100"/>
+      <c r="A23" s="88"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="57"/>
       <c r="F23" s="64" t="s">
         <v>330</v>
@@ -37264,10 +37264,10 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="92"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="100"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="57"/>
       <c r="F24" s="64" t="s">
         <v>333</v>
@@ -37292,10 +37292,10 @@
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="94"/>
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="104"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="102"/>
       <c r="E25" s="53"/>
       <c r="F25" s="64" t="s">
         <v>336</v>
@@ -37471,6 +37471,29 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="D22:D25"/>
     <mergeCell ref="A18:A19"/>
@@ -37480,29 +37503,6 @@
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -37536,7 +37536,9 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -37589,7 +37591,7 @@
       <c r="D2" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="E2" s="96" t="s">
+      <c r="E2" s="92" t="s">
         <v>366</v>
       </c>
       <c r="F2" s="43" t="s">
@@ -37603,7 +37605,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="92"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="43" t="s">
         <v>370</v>
       </c>
@@ -37613,17 +37615,17 @@
       <c r="D3" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="E3" s="94"/>
+      <c r="E3" s="99"/>
       <c r="F3" s="43" t="s">
         <v>373</v>
       </c>
       <c r="G3" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="H3" s="94"/>
+      <c r="H3" s="99"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="92"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="105" t="s">
         <v>375</v>
       </c>
@@ -37643,8 +37645,8 @@
       <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="92"/>
-      <c r="B5" s="94"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="43" t="s">
         <v>380</v>
       </c>
@@ -37660,8 +37662,8 @@
       </c>
       <c r="H5" s="21"/>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="92"/>
+    <row r="6" spans="1:8" ht="84" customHeight="1">
+      <c r="A6" s="88"/>
       <c r="B6" s="21" t="s">
         <v>384</v>
       </c>
@@ -37681,7 +37683,7 @@
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="94"/>
+      <c r="A7" s="99"/>
       <c r="B7" s="70" t="s">
         <v>388</v>
       </c>
@@ -37721,7 +37723,7 @@
       <c r="H9" s="64"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="90" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="80" t="s">
@@ -37741,7 +37743,7 @@
       <c r="H10" s="53"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="92"/>
+      <c r="A11" s="88"/>
       <c r="B11" s="49" t="s">
         <v>397</v>
       </c>
@@ -37759,7 +37761,7 @@
       <c r="H11" s="49"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="94"/>
+      <c r="A12" s="99"/>
       <c r="B12" s="49" t="s">
         <v>384</v>
       </c>

</xml_diff>